<commit_message>
adding working version for testing
</commit_message>
<xml_diff>
--- a/alpha_report.xlsx
+++ b/alpha_report.xlsx
@@ -1,32 +1,14 @@
-
-<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
-  <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-  </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
-</workbook>
-</file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +19,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +27,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -417,69 +390,4 @@
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
-</file>
-
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>provider_id</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>provider_name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>total_payments</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>average_monthly</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>growth_rate</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1001</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Alpha Payments</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>670000</v>
-      </c>
-      <c r="D2" t="n">
-        <v>167500</v>
-      </c>
-      <c r="E2" t="n">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Simplify scripts from demonstration of functionality
</commit_message>
<xml_diff>
--- a/alpha_report.xlsx
+++ b/alpha_report.xlsx
@@ -1,14 +1,34 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Summary" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Monthly Trends" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Distribution" sheetId="3" state="visible" r:id="rId3"/>
+  </sheets>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+</workbook>
+</file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -19,7 +39,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -27,12 +47,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -390,4 +419,228 @@
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>provider_id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>provider_name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>total_payments</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>avg_monthly_payment</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>highest_payment</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>lowest_payment</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>payment_fluctuation_pct</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Alpha Payments</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>670000</v>
+      </c>
+      <c r="D2" t="n">
+        <v>167500</v>
+      </c>
+      <c r="E2" t="n">
+        <v>180000</v>
+      </c>
+      <c r="F2" t="n">
+        <v>150000</v>
+      </c>
+      <c r="G2" t="n">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>month_number</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>payment_amount</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>growth_rate</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>150000</v>
+      </c>
+      <c r="C2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>165000</v>
+      </c>
+      <c r="C3" t="n">
+        <v>10.00000000000001</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>175000</v>
+      </c>
+      <c r="C4" t="n">
+        <v>6.060606060606055</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>180000</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2.857142857142847</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>provider_id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>provider_name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>num_months</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>months_above_avg</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>months_below_avg</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Alpha Payments</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>